<commit_message>
Alteração das Classes e Atualização dos Relatórios.
</commit_message>
<xml_diff>
--- a/resources/DicionarioDeDados.xlsx
+++ b/resources/DicionarioDeDados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>Pool</t>
   </si>
@@ -75,9 +75,6 @@
     <t>WorkflowProcess</t>
   </si>
   <si>
-    <t>Entidade representando o Elemento Lane.</t>
-  </si>
-  <si>
     <t>IdWorkflowProcess</t>
   </si>
   <si>
@@ -135,15 +132,9 @@
     <t>From</t>
   </si>
   <si>
-    <t>Atividade (Activity) Inicial. Indica de onde parte (Origem) da Transition (Conexão).</t>
-  </si>
-  <si>
     <t>To</t>
   </si>
   <si>
-    <t>Atividade (Activity) Final. Indica para onde vai (Destino) a Transition (Conexão).</t>
-  </si>
-  <si>
     <t>Indica o Tipo da Conexão de Condição.</t>
   </si>
   <si>
@@ -157,13 +148,77 @@
   </si>
   <si>
     <t>Nome da Pool.</t>
+  </si>
+  <si>
+    <t>Entidade representando o Elemento Lane. Uma Pool pode possuir várias Lanes.</t>
+  </si>
+  <si>
+    <t>ToolId</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>BorderColor</t>
+  </si>
+  <si>
+    <t>FillColor</t>
+  </si>
+  <si>
+    <t>BorderVisible</t>
+  </si>
+  <si>
+    <t>XCoordinate</t>
+  </si>
+  <si>
+    <t>YCoordinate</t>
+  </si>
+  <si>
+    <t>Id do Nome da Ferramenta de Modelagem.</t>
+  </si>
+  <si>
+    <t>Altura do Elemento.</t>
+  </si>
+  <si>
+    <t>Largura do Elemento.</t>
+  </si>
+  <si>
+    <t>Cor da Borda do Elemento.</t>
+  </si>
+  <si>
+    <t>Cor de Preenchimento do Elemento.</t>
+  </si>
+  <si>
+    <t>Indica se a Borda está visível ou não no Diagrama.</t>
+  </si>
+  <si>
+    <t>Indica o Ponto da Coordenada X onde o Elemento está posicionado.</t>
+  </si>
+  <si>
+    <t>Indica o Ponto da Coordenada Y onde o Elemento está posicionado.</t>
+  </si>
+  <si>
+    <t>UFMS | FACOM | Sistemas de Apoio à Decisão - 2013
+Trabalho - Mapeamento Relacional do BPMN 2.0
+Integrantes:
+- Heverson Silva Vasconcelos
+- Rodrigo Kuninari</t>
+  </si>
+  <si>
+    <t>Chave Estrangeira relacionando a Entidade Activity. Atividade Inicial. Indica de onde parte (Origem) da Transition (Conexão).</t>
+  </si>
+  <si>
+    <t>Chave Estrangeira relacionando a Entidade Activity. Atividade Final. Indica para onde vai (Destino) a Transition (Conexão).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +245,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -254,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -274,11 +336,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,290 +639,552 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="103.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:3" ht="90" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>3</v>
-      </c>
       <c r="C9" s="6" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
-        <v>13</v>
+      <c r="A10" s="8"/>
+      <c r="B10" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
-        <v>15</v>
+      <c r="A11" s="8"/>
+      <c r="B11" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>16</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
+      <c r="A13" s="8"/>
+      <c r="B13" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>3</v>
+      <c r="A14" s="8"/>
+      <c r="B14" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8" t="s">
-        <v>20</v>
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8" t="s">
-        <v>6</v>
+      <c r="A16" s="8"/>
+      <c r="B16" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="8"/>
+      <c r="B27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="8"/>
+      <c r="B29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="8"/>
+      <c r="B34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="6" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="7" t="s">
+      <c r="C38" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="8"/>
+      <c r="B41" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="C42" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="8"/>
+      <c r="B43" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="8"/>
+      <c r="B44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="8"/>
+      <c r="B45" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="8"/>
+      <c r="B46" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="8"/>
+      <c r="B47" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="8"/>
+      <c r="B48" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="8"/>
+      <c r="B49" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="C52" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="8"/>
+      <c r="B53" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="8"/>
+      <c r="B54" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="8"/>
+      <c r="B55" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="8"/>
+      <c r="B56" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8" t="s">
+      <c r="C56" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="8"/>
+      <c r="B57" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="7" t="s">
+      <c r="C57" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="8"/>
+      <c r="B58" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>43</v>
+      <c r="C58" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="8"/>
+      <c r="B59" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="8"/>
+      <c r="B60" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="8"/>
+      <c r="B61" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A26:A31"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:A16"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A37:A49"/>
+    <mergeCell ref="A52:A61"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.04" right="0.05" top="0.32" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>